<commit_message>
Rebuilt Enrollment and Registration Exe's
</commit_message>
<xml_diff>
--- a/Sample Data/Sample Personnel.xlsx
+++ b/Sample Data/Sample Personnel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\CBNHS-System\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CD4A69-0F5B-41B7-897D-5944DC47E8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FB82F1-76FD-4E2D-9509-CAD476462BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" firstSheet="1" activeTab="3" xr2:uid="{164A7487-796B-420C-87A6-5C41A14CB588}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" firstSheet="1" activeTab="4" xr2:uid="{164A7487-796B-420C-87A6-5C41A14CB588}"/>
   </bookViews>
   <sheets>
     <sheet name="Administrator (5)" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Department Head (2)" sheetId="4" r:id="rId4"/>
     <sheet name="Subject Teacher-Advisers (1)" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="98">
   <si>
     <t>Username</t>
   </si>
@@ -212,6 +212,117 @@
   </si>
   <si>
     <t>Dela Rosa</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Advisory 7</t>
+  </si>
+  <si>
+    <t>Advisory 8</t>
+  </si>
+  <si>
+    <t>Advisory 9</t>
+  </si>
+  <si>
+    <t>Advisory 10</t>
+  </si>
+  <si>
+    <t>English 7</t>
+  </si>
+  <si>
+    <t>English 8</t>
+  </si>
+  <si>
+    <t>English 9</t>
+  </si>
+  <si>
+    <t>English 10</t>
+  </si>
+  <si>
+    <t>Math 7</t>
+  </si>
+  <si>
+    <t>Math 9</t>
+  </si>
+  <si>
+    <t>Math 8</t>
+  </si>
+  <si>
+    <t>Math 10</t>
+  </si>
+  <si>
+    <t>Science 7</t>
+  </si>
+  <si>
+    <t>Science 8</t>
+  </si>
+  <si>
+    <t>Science 9</t>
+  </si>
+  <si>
+    <t>Science 10</t>
+  </si>
+  <si>
+    <t>Filipino 7</t>
+  </si>
+  <si>
+    <t>Filipino 8</t>
+  </si>
+  <si>
+    <t>Filipino 9</t>
+  </si>
+  <si>
+    <t>Filipino 10</t>
+  </si>
+  <si>
+    <t>AP 7</t>
+  </si>
+  <si>
+    <t>AP 8</t>
+  </si>
+  <si>
+    <t>AP 9</t>
+  </si>
+  <si>
+    <t>AP 10</t>
+  </si>
+  <si>
+    <t>ESP 7</t>
+  </si>
+  <si>
+    <t>ESP 8</t>
+  </si>
+  <si>
+    <t>ESP 9</t>
+  </si>
+  <si>
+    <t>ESP 10</t>
+  </si>
+  <si>
+    <t>TLE 7</t>
+  </si>
+  <si>
+    <t>TLE 8</t>
+  </si>
+  <si>
+    <t>TLE 9</t>
+  </si>
+  <si>
+    <t>TLE 10</t>
+  </si>
+  <si>
+    <t>MAPEH 7</t>
+  </si>
+  <si>
+    <t>MAPEH 8</t>
+  </si>
+  <si>
+    <t>MAPEH 9</t>
+  </si>
+  <si>
+    <t>MAPEH 10</t>
   </si>
 </sst>
 </file>
@@ -255,9 +366,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC04585E-7606-4EA9-AF0A-95DAE5D1F6BB}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,19 +1015,19 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F9" t="s">
@@ -921,44 +1035,70 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
       <c r="F10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
       <c r="F11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
       <c r="F12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
       <c r="F13" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E9:E13"/>
+    <mergeCell ref="D9:D13"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="A9:A13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F028F4-0468-479C-B19A-6AAA1C55B563}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -973,6 +1113,189 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Sample Personnel File
</commit_message>
<xml_diff>
--- a/Sample Data/Sample Personnel.xlsx
+++ b/Sample Data/Sample Personnel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\CBNHS-System\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FB82F1-76FD-4E2D-9509-CAD476462BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E360216-7EA6-46D6-B88F-6A25EEC71A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" firstSheet="1" activeTab="4" xr2:uid="{164A7487-796B-420C-87A6-5C41A14CB588}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="134">
   <si>
     <t>Username</t>
   </si>
@@ -323,6 +323,114 @@
   </si>
   <si>
     <t>MAPEH 10</t>
+  </si>
+  <si>
+    <t>Furahashi</t>
+  </si>
+  <si>
+    <t>Fumino</t>
+  </si>
+  <si>
+    <t>benkyu</t>
+  </si>
+  <si>
+    <t>Danny</t>
+  </si>
+  <si>
+    <t>Ash</t>
+  </si>
+  <si>
+    <t>Phantom</t>
+  </si>
+  <si>
+    <t>danny</t>
+  </si>
+  <si>
+    <t>Kal</t>
+  </si>
+  <si>
+    <t>Kent</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>superman</t>
+  </si>
+  <si>
+    <t>Kirisu</t>
+  </si>
+  <si>
+    <t>Mafuyu</t>
+  </si>
+  <si>
+    <t>Lynn</t>
+  </si>
+  <si>
+    <t>Haruka</t>
+  </si>
+  <si>
+    <t>mafuyu</t>
+  </si>
+  <si>
+    <t>Teodoro</t>
+  </si>
+  <si>
+    <t>Andal</t>
+  </si>
+  <si>
+    <t>Agoncillo</t>
+  </si>
+  <si>
+    <t>theodore</t>
+  </si>
+  <si>
+    <t>Nicomedes</t>
+  </si>
+  <si>
+    <t>Marquez</t>
+  </si>
+  <si>
+    <t>Joaquin</t>
+  </si>
+  <si>
+    <t>nick</t>
+  </si>
+  <si>
+    <t>Santa</t>
+  </si>
+  <si>
+    <t>Claus</t>
+  </si>
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Dalisay</t>
+  </si>
+  <si>
+    <t>Dela Cruz</t>
+  </si>
+  <si>
+    <t>juan</t>
+  </si>
+  <si>
+    <t>santa</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Gates</t>
+  </si>
+  <si>
+    <t>bill</t>
   </si>
 </sst>
 </file>
@@ -354,7 +462,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -362,16 +470,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1088,9 +1237,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F028F4-0468-479C-B19A-6AAA1C55B563}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1098,207 +1249,550 @@
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F2" t="s">
+      <c r="A2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F3" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F4" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F5" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
         <v>65</v>
       </c>
     </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
+      <c r="A7" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F8" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
         <v>69</v>
       </c>
     </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F15" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" t="s">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F25" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F27" t="s">
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F34" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F35" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F37" t="s">
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F38" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F39" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F40" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F42" t="s">
+    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F43" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F44" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F45" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4" t="s">
         <v>97</v>
       </c>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>